<commit_message>
significant work to get the API pull set up.
</commit_message>
<xml_diff>
--- a/FieldAnalysis.xlsx
+++ b/FieldAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Atharva/Documents/GitHub/NBA_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atharva\Documents\GitHub\NBA_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FC1A37-B7B1-FF40-AA58-21A70964E628}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE6D917-A379-47A4-B49A-111B48C8CBAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{1FE97ED2-D8CA-3443-B961-B13CF78D3B60}"/>
+    <workbookView xWindow="-37590" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{1FE97ED2-D8CA-3443-B961-B13CF78D3B60}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Tree and examples" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="Proposed tables" sheetId="3" r:id="rId3"/>
     <sheet name="Next steps" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="162">
   <si>
     <t>season</t>
   </si>
@@ -466,27 +464,18 @@
     <t>Season.Season</t>
   </si>
   <si>
-    <t>Team.TotalRecord</t>
-  </si>
-  <si>
     <t>not null, foreign key</t>
   </si>
   <si>
     <t>TeamID</t>
   </si>
   <si>
-    <t>Team.AverageRecord</t>
-  </si>
-  <si>
     <t>IsOpponent</t>
   </si>
   <si>
     <t>Player.Player</t>
   </si>
   <si>
-    <t>Player.TotalRecords</t>
-  </si>
-  <si>
     <t>PlayerID</t>
   </si>
   <si>
@@ -505,16 +494,31 @@
     <t>Need to create python script to pull from the API.</t>
   </si>
   <si>
-    <t xml:space="preserve">Shouldn't be that hard, but want to save the pulled XMLs somewhere local so we can use them afterwards. </t>
-  </si>
-  <si>
-    <t>Needs to pull 1 per team per year so that’s 30 * (max) 7?</t>
-  </si>
-  <si>
     <t>Then, need to figure out how to analyze the data</t>
   </si>
   <si>
     <t>Need to create python script to pull from XMLs into a SQL table / schema or figure out how to drop it into a nice CSV</t>
+  </si>
+  <si>
+    <t>Need to pull 1 per team per year so that’s 30 * (max) 7?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shouldn't be that hard, but also want to save the pulled XMLs somewhere local so we can use them afterwards. </t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>Player.Average</t>
+  </si>
+  <si>
+    <t>Player.Total</t>
+  </si>
+  <si>
+    <t>Team.Average</t>
+  </si>
+  <si>
+    <t>Team.Total</t>
   </si>
 </sst>
 </file>
@@ -1053,24 +1057,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A54828-9529-AB49-8E2C-D44735EFFA34}">
   <dimension ref="A1:K312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="H283" sqref="H283"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H297" sqref="H297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>74</v>
       </c>
@@ -1129,7 +1133,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>75</v>
       </c>
@@ -1159,7 +1163,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>76</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -1204,7 +1208,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>77</v>
       </c>
@@ -1219,7 +1223,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>78</v>
       </c>
@@ -1234,7 +1238,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>15</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>16</v>
       </c>
@@ -1264,7 +1268,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>72</v>
       </c>
@@ -1280,7 +1284,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
         <v>2</v>
@@ -1296,7 +1300,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -1313,7 +1317,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1328,7 +1332,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1343,7 +1347,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1358,7 +1362,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1373,7 +1377,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1388,7 +1392,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1403,7 +1407,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1418,7 +1422,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1433,7 +1437,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1448,7 +1452,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1463,7 +1467,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1478,7 +1482,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1493,7 +1497,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1508,7 +1512,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1523,7 +1527,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1538,7 +1542,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1553,7 +1557,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1568,7 +1572,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1583,7 +1587,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1598,7 +1602,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1613,7 +1617,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1628,7 +1632,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1643,7 +1647,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1658,7 +1662,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1673,7 +1677,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1688,7 +1692,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1703,7 +1707,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1718,7 +1722,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1733,7 +1737,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1748,7 +1752,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1763,7 +1767,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1778,7 +1782,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1793,7 +1797,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1808,7 +1812,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1823,7 +1827,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1838,7 +1842,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1853,7 +1857,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1868,7 +1872,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -1883,7 +1887,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1898,7 +1902,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1913,7 +1917,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1928,7 +1932,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -1943,7 +1947,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -1958,7 +1962,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -1973,7 +1977,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -1988,7 +1992,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -2003,7 +2007,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2018,7 +2022,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -2033,7 +2037,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -2048,7 +2052,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -2063,7 +2067,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -2078,7 +2082,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -2093,7 +2097,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2108,7 +2112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -2123,7 +2127,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -2138,7 +2142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -2153,7 +2157,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -2168,7 +2172,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -2183,7 +2187,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -2198,7 +2202,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -2213,7 +2217,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
@@ -2230,7 +2234,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2245,7 +2249,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -2260,7 +2264,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -2275,7 +2279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -2290,7 +2294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -2305,7 +2309,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -2320,7 +2324,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -2335,7 +2339,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -2350,7 +2354,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -2365,7 +2369,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -2380,7 +2384,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -2395,7 +2399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -2410,7 +2414,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -2425,7 +2429,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -2440,7 +2444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -2455,7 +2459,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -2470,7 +2474,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -2485,7 +2489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -2500,7 +2504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -2515,7 +2519,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -2530,7 +2534,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -2545,7 +2549,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -2560,7 +2564,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -2575,7 +2579,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -2590,7 +2594,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -2605,7 +2609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -2620,7 +2624,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -2635,7 +2639,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -2650,7 +2654,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -2665,7 +2669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -2680,7 +2684,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -2695,7 +2699,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -2710,7 +2714,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -2725,7 +2729,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -2740,7 +2744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -2755,7 +2759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
         <v>115</v>
@@ -2771,7 +2775,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="113" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1" t="s">
@@ -2788,7 +2792,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="114" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -2803,7 +2807,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="115" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -2818,7 +2822,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -2833,7 +2837,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="117" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -2848,7 +2852,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="118" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -2863,7 +2867,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -2878,7 +2882,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="120" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -2893,7 +2897,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -2908,7 +2912,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -2923,7 +2927,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="123" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -2938,7 +2942,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="124" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
@@ -2953,7 +2957,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -2968,7 +2972,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="126" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -2983,7 +2987,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="127" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -2998,7 +3002,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="128" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -3013,7 +3017,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -3028,7 +3032,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="130" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -3043,7 +3047,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="131" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -3058,7 +3062,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="132" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -3073,7 +3077,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="133" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -3088,7 +3092,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="134" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -3103,7 +3107,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -3118,7 +3122,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -3133,7 +3137,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="137" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -3148,7 +3152,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="138" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
@@ -3163,7 +3167,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="139" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -3178,7 +3182,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="140" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
@@ -3193,7 +3197,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="141" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -3208,7 +3212,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="142" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -3223,7 +3227,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="143" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -3238,7 +3242,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="144" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -3253,7 +3257,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="145" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -3268,7 +3272,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="146" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -3283,7 +3287,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="147" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -3298,7 +3302,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="148" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -3313,7 +3317,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="149" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -3328,7 +3332,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="150" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -3343,7 +3347,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="151" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -3358,7 +3362,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="152" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -3373,7 +3377,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="153" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -3388,7 +3392,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="154" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -3403,7 +3407,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="155" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -3418,7 +3422,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="156" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
@@ -3433,7 +3437,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="157" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
@@ -3448,7 +3452,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
@@ -3463,7 +3467,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="159" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
@@ -3478,7 +3482,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="160" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
@@ -3493,7 +3497,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="161" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -3508,7 +3512,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="162" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -3523,7 +3527,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="163" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -3538,7 +3542,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="164" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -3553,7 +3557,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="165" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -3568,7 +3572,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="166" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -3583,7 +3587,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="167" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
@@ -3598,7 +3602,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="168" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
@@ -3613,7 +3617,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="169" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
@@ -3628,7 +3632,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="170" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
@@ -3643,7 +3647,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="171" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
@@ -3658,7 +3662,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="172" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
@@ -3673,7 +3677,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="173" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -3688,7 +3692,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="174" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1" t="s">
@@ -3705,7 +3709,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="175" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -3720,7 +3724,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="176" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -3735,7 +3739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="177" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
@@ -3750,7 +3754,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="178" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -3765,7 +3769,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="179" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
@@ -3780,7 +3784,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="180" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
@@ -3795,7 +3799,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="181" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -3810,7 +3814,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="182" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -3825,7 +3829,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="183" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -3840,7 +3844,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="184" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -3855,7 +3859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="185" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -3870,7 +3874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="186" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
@@ -3885,7 +3889,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="187" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -3900,7 +3904,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="188" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
@@ -3915,7 +3919,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="189" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
@@ -3930,7 +3934,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="190" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -3945,7 +3949,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="191" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
@@ -3960,7 +3964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="192" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
@@ -3975,7 +3979,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="193" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
@@ -3990,7 +3994,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="194" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -4005,7 +4009,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="195" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -4020,7 +4024,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="196" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
@@ -4035,7 +4039,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="197" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -4050,7 +4054,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="198" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
@@ -4065,7 +4069,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="199" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
@@ -4080,7 +4084,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="200" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -4095,7 +4099,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="201" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
@@ -4110,7 +4114,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="202" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -4125,7 +4129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="203" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
@@ -4140,7 +4144,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="204" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
@@ -4155,7 +4159,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="205" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -4170,7 +4174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="206" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -4185,7 +4189,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="207" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -4200,7 +4204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="208" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
@@ -4215,7 +4219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="209" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
@@ -4230,7 +4234,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="210" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C210" s="1" t="s">
         <v>73</v>
       </c>
@@ -4246,7 +4250,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="211" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
         <v>2</v>
@@ -4262,7 +4266,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="212" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C212" s="1"/>
       <c r="E212" s="1" t="s">
         <v>8</v>
@@ -4278,7 +4282,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="213" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C213" s="1"/>
       <c r="E213" s="1"/>
       <c r="F213" t="s">
@@ -4292,7 +4296,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="214" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C214" s="1"/>
       <c r="E214" s="1"/>
       <c r="F214" t="s">
@@ -4306,7 +4310,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="215" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C215" s="1"/>
       <c r="E215" s="1"/>
       <c r="F215" t="s">
@@ -4320,7 +4324,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="216" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C216" s="1"/>
       <c r="E216" s="1"/>
       <c r="F216" t="s">
@@ -4334,7 +4338,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="217" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C217" s="1"/>
       <c r="E217" s="1"/>
       <c r="F217" t="s">
@@ -4348,7 +4352,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="218" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C218" s="1"/>
       <c r="E218" s="1"/>
       <c r="F218" t="s">
@@ -4362,7 +4366,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="219" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C219" s="1"/>
       <c r="E219" s="1"/>
       <c r="F219" t="s">
@@ -4376,7 +4380,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="220" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C220" s="1"/>
       <c r="E220" s="1"/>
       <c r="F220" t="s">
@@ -4396,7 +4400,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="221" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C221" s="1"/>
       <c r="E221" s="1"/>
       <c r="F221" t="s">
@@ -4416,7 +4420,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="222" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C222" s="1"/>
       <c r="E222" s="1" t="s">
         <v>3</v>
@@ -4432,7 +4436,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="223" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C223" s="1"/>
       <c r="E223" s="1"/>
       <c r="F223" t="s">
@@ -4447,7 +4451,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="224" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:11" x14ac:dyDescent="0.25">
       <c r="F224" t="s">
         <v>18</v>
       </c>
@@ -4459,7 +4463,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="225" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="225" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F225" t="s">
         <v>6</v>
       </c>
@@ -4471,7 +4475,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="226" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="226" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F226" t="s">
         <v>7</v>
       </c>
@@ -4483,7 +4487,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="227" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="227" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F227" t="s">
         <v>19</v>
       </c>
@@ -4495,7 +4499,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="228" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F228" t="s">
         <v>20</v>
       </c>
@@ -4507,7 +4511,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="229" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="229" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F229" t="s">
         <v>21</v>
       </c>
@@ -4519,7 +4523,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="230" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="230" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F230" t="s">
         <v>22</v>
       </c>
@@ -4531,7 +4535,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="231" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="231" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F231" t="s">
         <v>23</v>
       </c>
@@ -4543,7 +4547,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="232" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="232" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F232" t="s">
         <v>24</v>
       </c>
@@ -4555,7 +4559,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="233" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="233" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F233" t="s">
         <v>25</v>
       </c>
@@ -4567,7 +4571,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="234" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="234" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F234" t="s">
         <v>26</v>
       </c>
@@ -4579,7 +4583,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="235" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="235" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F235" t="s">
         <v>27</v>
       </c>
@@ -4591,7 +4595,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="236" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="236" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F236" t="s">
         <v>28</v>
       </c>
@@ -4603,7 +4607,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="237" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="237" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F237" t="s">
         <v>29</v>
       </c>
@@ -4615,7 +4619,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="238" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="238" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F238" t="s">
         <v>30</v>
       </c>
@@ -4627,7 +4631,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="239" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="239" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F239" t="s">
         <v>31</v>
       </c>
@@ -4639,7 +4643,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="240" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="240" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F240" t="s">
         <v>32</v>
       </c>
@@ -4651,7 +4655,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="241" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="241" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F241" t="s">
         <v>33</v>
       </c>
@@ -4663,7 +4667,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="242" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="242" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F242" t="s">
         <v>34</v>
       </c>
@@ -4675,7 +4679,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="243" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="243" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F243" t="s">
         <v>35</v>
       </c>
@@ -4687,7 +4691,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="244" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="244" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F244" t="s">
         <v>36</v>
       </c>
@@ -4699,7 +4703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="245" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="245" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F245" t="s">
         <v>37</v>
       </c>
@@ -4711,7 +4715,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="246" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="246" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F246" t="s">
         <v>38</v>
       </c>
@@ -4723,7 +4727,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="247" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="247" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F247" t="s">
         <v>39</v>
       </c>
@@ -4735,7 +4739,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="248" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="248" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F248" t="s">
         <v>40</v>
       </c>
@@ -4747,7 +4751,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="249" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="249" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F249" t="s">
         <v>41</v>
       </c>
@@ -4759,7 +4763,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="250" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="250" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F250" t="s">
         <v>42</v>
       </c>
@@ -4771,7 +4775,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="251" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="251" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F251" t="s">
         <v>43</v>
       </c>
@@ -4783,7 +4787,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="252" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="252" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F252" t="s">
         <v>44</v>
       </c>
@@ -4795,7 +4799,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="253" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="253" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F253" t="s">
         <v>45</v>
       </c>
@@ -4807,7 +4811,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="254" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="254" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F254" t="s">
         <v>46</v>
       </c>
@@ -4819,7 +4823,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="255" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="255" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F255" t="s">
         <v>47</v>
       </c>
@@ -4831,7 +4835,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="256" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="256" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F256" t="s">
         <v>48</v>
       </c>
@@ -4843,7 +4847,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="257" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="257" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F257" t="s">
         <v>49</v>
       </c>
@@ -4855,7 +4859,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="258" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="258" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F258" t="s">
         <v>50</v>
       </c>
@@ -4867,7 +4871,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="259" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="259" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F259" t="s">
         <v>51</v>
       </c>
@@ -4879,7 +4883,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="260" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="260" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F260" t="s">
         <v>52</v>
       </c>
@@ -4891,7 +4895,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="261" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="261" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F261" t="s">
         <v>53</v>
       </c>
@@ -4903,7 +4907,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="262" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="262" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F262" t="s">
         <v>54</v>
       </c>
@@ -4915,7 +4919,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="263" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="263" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F263" t="s">
         <v>55</v>
       </c>
@@ -4927,7 +4931,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="264" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="264" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F264" t="s">
         <v>56</v>
       </c>
@@ -4939,7 +4943,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="265" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="265" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F265" t="s">
         <v>57</v>
       </c>
@@ -4951,7 +4955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="266" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="266" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F266" t="s">
         <v>58</v>
       </c>
@@ -4963,7 +4967,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="267" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="267" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F267" t="s">
         <v>59</v>
       </c>
@@ -4975,7 +4979,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="268" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="268" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F268" t="s">
         <v>60</v>
       </c>
@@ -4987,7 +4991,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="269" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="269" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F269" t="s">
         <v>61</v>
       </c>
@@ -4999,7 +5003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="270" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="270" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F270" t="s">
         <v>62</v>
       </c>
@@ -5011,7 +5015,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="271" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="271" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F271" t="s">
         <v>63</v>
       </c>
@@ -5023,7 +5027,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="272" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="272" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F272" t="s">
         <v>64</v>
       </c>
@@ -5035,7 +5039,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="273" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="273" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F273" t="s">
         <v>65</v>
       </c>
@@ -5047,7 +5051,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="274" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="274" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F274" t="s">
         <v>66</v>
       </c>
@@ -5059,7 +5063,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="275" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="275" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F275" t="s">
         <v>67</v>
       </c>
@@ -5071,7 +5075,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="276" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="276" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F276" t="s">
         <v>68</v>
       </c>
@@ -5083,7 +5087,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="277" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="277" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F277" t="s">
         <v>69</v>
       </c>
@@ -5095,7 +5099,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="278" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="278" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E278" s="1" t="s">
         <v>4</v>
       </c>
@@ -5110,7 +5114,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="279" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="279" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F279" t="s">
         <v>6</v>
       </c>
@@ -5125,7 +5129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="280" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="280" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F280" t="s">
         <v>41</v>
       </c>
@@ -5140,7 +5144,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="281" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="281" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F281" t="s">
         <v>70</v>
       </c>
@@ -5155,7 +5159,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="282" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="282" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F282" t="s">
         <v>71</v>
       </c>
@@ -5170,7 +5174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="283" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="283" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F283" t="s">
         <v>33</v>
       </c>
@@ -5185,7 +5189,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="284" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="284" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F284" t="s">
         <v>34</v>
       </c>
@@ -5200,7 +5204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="285" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="285" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F285" t="s">
         <v>37</v>
       </c>
@@ -5215,7 +5219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="286" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="286" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F286" t="s">
         <v>38</v>
       </c>
@@ -5230,7 +5234,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="287" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="287" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F287" t="s">
         <v>35</v>
       </c>
@@ -5245,7 +5249,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="288" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="288" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F288" t="s">
         <v>39</v>
       </c>
@@ -5260,7 +5264,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="289" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="289" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F289" t="s">
         <v>42</v>
       </c>
@@ -5275,7 +5279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="290" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="290" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F290" t="s">
         <v>27</v>
       </c>
@@ -5290,7 +5294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="291" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="291" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F291" t="s">
         <v>7</v>
       </c>
@@ -5305,7 +5309,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="292" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="292" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F292" t="s">
         <v>19</v>
       </c>
@@ -5320,7 +5324,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="293" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="293" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F293" t="s">
         <v>24</v>
       </c>
@@ -5335,7 +5339,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="294" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="294" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F294" t="s">
         <v>25</v>
       </c>
@@ -5350,7 +5354,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="295" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="295" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F295" t="s">
         <v>28</v>
       </c>
@@ -5365,7 +5369,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="296" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="296" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F296" t="s">
         <v>29</v>
       </c>
@@ -5380,7 +5384,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="297" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="297" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F297" t="s">
         <v>21</v>
       </c>
@@ -5395,7 +5399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="298" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="298" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F298" t="s">
         <v>22</v>
       </c>
@@ -5410,7 +5414,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="299" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="299" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F299" t="s">
         <v>47</v>
       </c>
@@ -5425,7 +5429,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="300" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="300" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F300" t="s">
         <v>45</v>
       </c>
@@ -5440,7 +5444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="301" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="301" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F301" t="s">
         <v>48</v>
       </c>
@@ -5455,7 +5459,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="302" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="302" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F302" t="s">
         <v>50</v>
       </c>
@@ -5470,7 +5474,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="303" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="303" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F303" t="s">
         <v>51</v>
       </c>
@@ -5485,7 +5489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="304" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="304" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F304" t="s">
         <v>49</v>
       </c>
@@ -5500,7 +5504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="305" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="305" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F305" t="s">
         <v>56</v>
       </c>
@@ -5515,7 +5519,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="306" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="306" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F306" t="s">
         <v>57</v>
       </c>
@@ -5530,7 +5534,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="307" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="307" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F307" t="s">
         <v>58</v>
       </c>
@@ -5545,7 +5549,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="308" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="308" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F308" t="s">
         <v>59</v>
       </c>
@@ -5560,7 +5564,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="309" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="309" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F309" t="s">
         <v>60</v>
       </c>
@@ -5575,7 +5579,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="310" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="310" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F310" t="s">
         <v>64</v>
       </c>
@@ -5590,7 +5594,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="311" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="311" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F311" t="s">
         <v>65</v>
       </c>
@@ -5605,7 +5609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="312" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="312" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F312" t="s">
         <v>66</v>
       </c>
@@ -5622,6 +5626,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5629,67 +5634,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A95B3A-52DF-1748-B037-EEA495CFFFA6}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="R2" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="15" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="19.625" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="17.5" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="15" bestFit="1" customWidth="1"/>
     <col min="45" max="47" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="17.125" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="17" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="17" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="10.5" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="13.5" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5871,12 +5876,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -5983,12 +5988,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -6155,12 +6160,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -6266,38 +6271,39 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8F9D3B-E9AA-B143-B309-156157DA3304}">
-  <dimension ref="B2:P78"/>
+  <dimension ref="B2:P82"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N55" sqref="N22:N55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>142</v>
       </c>
@@ -6309,7 +6315,7 @@
       <c r="G2" s="28"/>
       <c r="H2" s="29"/>
       <c r="J2" s="27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="29"/>
@@ -6319,7 +6325,7 @@
       <c r="O2" s="25"/>
       <c r="P2" s="26"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>118</v>
       </c>
@@ -6357,12 +6363,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>135</v>
@@ -6371,7 +6377,7 @@
         <v>119</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>135</v>
@@ -6380,7 +6386,7 @@
         <v>119</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>135</v>
@@ -6389,18 +6395,18 @@
         <v>119</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>120</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D5" s="7"/>
       <c r="F5" s="5" t="s">
@@ -6411,23 +6417,23 @@
       </c>
       <c r="H5" s="7"/>
       <c r="J5" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L5" s="7"/>
       <c r="N5" s="5" t="s">
         <v>126</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>121</v>
       </c>
@@ -6459,7 +6465,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>123</v>
       </c>
@@ -6473,7 +6479,7 @@
         <v>120</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="H7" s="7"/>
       <c r="J7" s="5" t="s">
@@ -6493,7 +6499,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>125</v>
       </c>
@@ -6504,19 +6510,19 @@
         <v>133</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>120</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L8" s="7"/>
       <c r="N8" s="5" t="s">
@@ -6529,7 +6535,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>139</v>
       </c>
@@ -6563,7 +6569,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F10" s="5" t="s">
         <v>137</v>
       </c>
@@ -6583,41 +6589,41 @@
         <v>138</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="P10" s="20" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F11" s="5" t="s">
         <v>140</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="H11" s="7"/>
       <c r="J11" s="5" t="s">
         <v>140</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L11" s="7"/>
       <c r="N11" s="8" t="s">
         <v>131</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="P11" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F12" s="8" t="s">
         <v>139</v>
       </c>
@@ -6627,69 +6633,69 @@
         <v>13</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J15" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K15" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J16" s="8" t="s">
         <v>139</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="10"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="27" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
       <c r="F18" s="27" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="G18" s="28"/>
       <c r="H18" s="29"/>
       <c r="J18" s="21" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="K18" s="22"/>
       <c r="L18" s="23"/>
       <c r="N18" s="21" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="O18" s="22"/>
       <c r="P18" s="23"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>118</v>
       </c>
@@ -6727,12 +6733,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>91</v>
+      <c r="C20" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>135</v>
@@ -6741,7 +6747,7 @@
         <v>119</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>135</v>
@@ -6750,7 +6756,7 @@
         <v>119</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L20" s="13" t="s">
         <v>135</v>
@@ -6759,70 +6765,70 @@
         <v>119</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="P20" s="13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="G21" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D22" s="7"/>
       <c r="F22" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="H22" s="7"/>
       <c r="J22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L22" s="7"/>
       <c r="N22" s="5" t="s">
@@ -6833,9 +6839,9 @@
       </c>
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>100</v>
@@ -6852,7 +6858,7 @@
         <v>18</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L23" s="7"/>
       <c r="N23" s="5" t="s">
@@ -6863,12 +6869,12 @@
       </c>
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D24" s="7"/>
       <c r="F24" s="18" t="s">
@@ -6882,7 +6888,7 @@
         <v>6</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L24" s="7"/>
       <c r="N24" s="5" t="s">
@@ -6893,12 +6899,12 @@
       </c>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D25" s="7"/>
       <c r="F25" s="18" t="s">
@@ -6912,7 +6918,7 @@
         <v>7</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L25" s="7"/>
       <c r="N25" s="5" t="s">
@@ -6923,9 +6929,9 @@
       </c>
       <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>100</v>
@@ -6942,7 +6948,7 @@
         <v>19</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L26" s="7"/>
       <c r="N26" s="5" t="s">
@@ -6953,12 +6959,12 @@
       </c>
       <c r="P26" s="7"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D27" s="7"/>
       <c r="F27" s="18" t="s">
@@ -6983,12 +6989,12 @@
       </c>
       <c r="P27" s="7"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D28" s="7"/>
       <c r="F28" s="18" t="s">
@@ -7002,7 +7008,7 @@
         <v>21</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L28" s="7"/>
       <c r="N28" s="5" t="s">
@@ -7013,9 +7019,9 @@
       </c>
       <c r="P28" s="7"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>100</v>
@@ -7032,7 +7038,7 @@
         <v>22</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L29" s="7"/>
       <c r="N29" s="5" t="s">
@@ -7043,12 +7049,12 @@
       </c>
       <c r="P29" s="7"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D30" s="7"/>
       <c r="F30" s="18" t="s">
@@ -7073,12 +7079,12 @@
       </c>
       <c r="P30" s="7"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D31" s="7"/>
       <c r="F31" s="18" t="s">
@@ -7092,7 +7098,7 @@
         <v>24</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L31" s="7"/>
       <c r="N31" s="5" t="s">
@@ -7103,9 +7109,9 @@
       </c>
       <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>100</v>
@@ -7122,7 +7128,7 @@
         <v>25</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L32" s="7"/>
       <c r="N32" s="5" t="s">
@@ -7133,12 +7139,12 @@
       </c>
       <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D33" s="7"/>
       <c r="F33" s="18" t="s">
@@ -7163,12 +7169,12 @@
       </c>
       <c r="P33" s="7"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D34" s="7"/>
       <c r="F34" s="18" t="s">
@@ -7182,7 +7188,7 @@
         <v>27</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L34" s="7"/>
       <c r="N34" s="5" t="s">
@@ -7193,12 +7199,12 @@
       </c>
       <c r="P34" s="7"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D35" s="7"/>
       <c r="F35" s="18" t="s">
@@ -7212,7 +7218,7 @@
         <v>28</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L35" s="7"/>
       <c r="N35" s="5" t="s">
@@ -7223,9 +7229,9 @@
       </c>
       <c r="P35" s="7"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>100</v>
@@ -7242,7 +7248,7 @@
         <v>29</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L36" s="7"/>
       <c r="N36" s="5" t="s">
@@ -7253,12 +7259,12 @@
       </c>
       <c r="P36" s="7"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D37" s="7"/>
       <c r="F37" s="18" t="s">
@@ -7283,12 +7289,12 @@
       </c>
       <c r="P37" s="7"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D38" s="7"/>
       <c r="F38" s="18" t="s">
@@ -7302,7 +7308,7 @@
         <v>31</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L38" s="7"/>
       <c r="N38" s="5" t="s">
@@ -7313,12 +7319,12 @@
       </c>
       <c r="P38" s="7"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D39" s="7"/>
       <c r="F39" s="18" t="s">
@@ -7332,7 +7338,7 @@
         <v>32</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L39" s="7"/>
       <c r="N39" s="5" t="s">
@@ -7343,12 +7349,12 @@
       </c>
       <c r="P39" s="7"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D40" s="7"/>
       <c r="F40" s="18" t="s">
@@ -7362,7 +7368,7 @@
         <v>33</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L40" s="7"/>
       <c r="N40" s="5" t="s">
@@ -7373,12 +7379,12 @@
       </c>
       <c r="P40" s="7"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D41" s="7"/>
       <c r="F41" s="18" t="s">
@@ -7392,7 +7398,7 @@
         <v>34</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L41" s="7"/>
       <c r="N41" s="5" t="s">
@@ -7403,9 +7409,9 @@
       </c>
       <c r="P41" s="7"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>100</v>
@@ -7422,7 +7428,7 @@
         <v>35</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L42" s="7"/>
       <c r="N42" s="5" t="s">
@@ -7433,12 +7439,12 @@
       </c>
       <c r="P42" s="7"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D43" s="7"/>
       <c r="F43" s="18" t="s">
@@ -7463,12 +7469,12 @@
       </c>
       <c r="P43" s="7"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D44" s="7"/>
       <c r="F44" s="18" t="s">
@@ -7482,7 +7488,7 @@
         <v>37</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L44" s="7"/>
       <c r="N44" s="5" t="s">
@@ -7493,12 +7499,12 @@
       </c>
       <c r="P44" s="7"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D45" s="7"/>
       <c r="F45" s="18" t="s">
@@ -7512,7 +7518,7 @@
         <v>38</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L45" s="7"/>
       <c r="N45" s="5" t="s">
@@ -7523,12 +7529,12 @@
       </c>
       <c r="P45" s="7"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D46" s="7"/>
       <c r="F46" s="18" t="s">
@@ -7542,7 +7548,7 @@
         <v>39</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L46" s="7"/>
       <c r="N46" s="5" t="s">
@@ -7553,12 +7559,12 @@
       </c>
       <c r="P46" s="7"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D47" s="7"/>
       <c r="F47" s="18" t="s">
@@ -7572,7 +7578,7 @@
         <v>40</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L47" s="7"/>
       <c r="N47" s="5" t="s">
@@ -7583,12 +7589,12 @@
       </c>
       <c r="P47" s="7"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D48" s="7"/>
       <c r="F48" s="18" t="s">
@@ -7602,7 +7608,7 @@
         <v>41</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L48" s="7"/>
       <c r="N48" s="5" t="s">
@@ -7613,12 +7619,12 @@
       </c>
       <c r="P48" s="7"/>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D49" s="7"/>
       <c r="F49" s="18" t="s">
@@ -7632,7 +7638,7 @@
         <v>42</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L49" s="7"/>
       <c r="N49" s="5" t="s">
@@ -7643,12 +7649,12 @@
       </c>
       <c r="P49" s="7"/>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D50" s="7"/>
       <c r="F50" s="18" t="s">
@@ -7662,7 +7668,7 @@
         <v>43</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L50" s="7"/>
       <c r="N50" s="5" t="s">
@@ -7673,12 +7679,12 @@
       </c>
       <c r="P50" s="7"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D51" s="7"/>
       <c r="F51" s="18" t="s">
@@ -7692,7 +7698,7 @@
         <v>44</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L51" s="7"/>
       <c r="N51" s="5" t="s">
@@ -7703,12 +7709,12 @@
       </c>
       <c r="P51" s="7"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D52" s="7"/>
       <c r="F52" s="18" t="s">
@@ -7722,7 +7728,7 @@
         <v>45</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L52" s="7"/>
       <c r="N52" s="5" t="s">
@@ -7733,12 +7739,12 @@
       </c>
       <c r="P52" s="7"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D53" s="7"/>
       <c r="F53" s="18" t="s">
@@ -7763,12 +7769,12 @@
       </c>
       <c r="P53" s="7"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D54" s="7"/>
       <c r="F54" s="18" t="s">
@@ -7782,7 +7788,7 @@
         <v>47</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L54" s="7"/>
       <c r="N54" s="5" t="s">
@@ -7793,12 +7799,12 @@
       </c>
       <c r="P54" s="7"/>
     </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D55" s="7"/>
       <c r="F55" s="18" t="s">
@@ -7812,7 +7818,7 @@
         <v>48</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L55" s="7"/>
       <c r="N55" s="5" t="s">
@@ -7823,12 +7829,12 @@
       </c>
       <c r="P55" s="7"/>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D56" s="7"/>
       <c r="F56" s="18" t="s">
@@ -7842,7 +7848,7 @@
         <v>49</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L56" s="7"/>
       <c r="N56" s="8" t="s">
@@ -7851,9 +7857,9 @@
       <c r="O56" s="9"/>
       <c r="P56" s="10"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>100</v>
@@ -7870,16 +7876,16 @@
         <v>50</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L57" s="7"/>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D58" s="7"/>
       <c r="F58" s="8" t="s">
@@ -7891,16 +7897,16 @@
         <v>51</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L58" s="7"/>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D59" s="7"/>
       <c r="J59" s="5" t="s">
@@ -7911,12 +7917,12 @@
       </c>
       <c r="L59" s="7"/>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D60" s="7"/>
       <c r="J60" s="5" t="s">
@@ -7927,124 +7933,124 @@
       </c>
       <c r="L60" s="7"/>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D61" s="7"/>
       <c r="J61" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L61" s="7"/>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D62" s="7"/>
       <c r="J62" s="5" t="s">
         <v>55</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L62" s="7"/>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D63" s="7"/>
       <c r="J63" s="5" t="s">
         <v>56</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L63" s="7"/>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D64" s="7"/>
       <c r="J64" s="5" t="s">
         <v>57</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L64" s="7"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="D65" s="7"/>
       <c r="J65" s="5" t="s">
         <v>58</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L65" s="7"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D66" s="7"/>
       <c r="J66" s="5" t="s">
         <v>59</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L66" s="7"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D67" s="7"/>
       <c r="J67" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K67" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L67" s="7"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D68" s="7"/>
       <c r="J68" s="5" t="s">
@@ -8055,28 +8061,28 @@
       </c>
       <c r="L68" s="7"/>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D69" s="7"/>
       <c r="J69" s="5" t="s">
         <v>62</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L69" s="7"/>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D70" s="7"/>
       <c r="J70" s="5" t="s">
@@ -8087,108 +8093,108 @@
       </c>
       <c r="L70" s="7"/>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D71" s="7"/>
       <c r="J71" s="5" t="s">
         <v>64</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L71" s="7"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D72" s="7"/>
       <c r="J72" s="5" t="s">
         <v>65</v>
       </c>
       <c r="K72" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L72" s="7"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="D73" s="7"/>
       <c r="J73" s="5" t="s">
         <v>66</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L73" s="7"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D74" s="7"/>
       <c r="J74" s="5" t="s">
         <v>67</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L74" s="7"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D75" s="7"/>
       <c r="J75" s="5" t="s">
         <v>68</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L75" s="7"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="D76" s="7"/>
       <c r="J76" s="5" t="s">
         <v>69</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="L76" s="7"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B77" s="8" t="s">
-        <v>139</v>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D77" s="7"/>
       <c r="J77" s="8" t="s">
@@ -8197,9 +8203,48 @@
       <c r="K77" s="9"/>
       <c r="L77" s="10"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C78" s="9"/>
-      <c r="D78" s="10"/>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D81" s="7"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" s="9"/>
+      <c r="D82" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -8213,6 +8258,8 @@
     <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <picture r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8221,37 +8268,38 @@
   <dimension ref="A2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some comments. cleaned up a little
</commit_message>
<xml_diff>
--- a/FieldAnalysis.xlsx
+++ b/FieldAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atharva\Documents\GitHub\NBA_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE6D917-A379-47A4-B49A-111B48C8CBAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED531288-8264-4C8E-A1F4-6F169F432AC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37590" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{1FE97ED2-D8CA-3443-B961-B13CF78D3B60}"/>
+    <workbookView xWindow="-37590" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="2" xr2:uid="{1FE97ED2-D8CA-3443-B961-B13CF78D3B60}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Tree and examples" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="217">
   <si>
     <t>season</t>
   </si>
@@ -519,6 +519,171 @@
   </si>
   <si>
     <t>Team.Total</t>
+  </si>
+  <si>
+    <t>['games_played'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'games_started'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'minutes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'field_goals_made'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'field_goals_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'field_goals_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'two_points_made'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'two_points_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'two_points_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'three_points_made'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'three_points_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'three_points_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'blocked_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'free_throws_made'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'free_throws_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'free_throws_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'offensive_rebounds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'defensive_rebounds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'rebounds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'assists'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'turnovers'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'assists_turnover_ratio'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'steals'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'blocks'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'personal_fouls'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'tech_fouls'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'points'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'flagrant_fouls'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ejections'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'foulouts'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'true_shooting_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'true_shooting_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'efficiency'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'points_off_turnovers'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'points_in_paint'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'points_in_paint_made'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'points_in_paint_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'points_in_paint_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'effective_fg_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'double_doubles'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'triple_doubles'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fouls_drawn'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'offensive_fouls'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fast_break_pts'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fast_break_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fast_break_made'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fast_break_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'coach_ejections'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'second_chance_pct'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'second_chance_pts'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'second_chance_att'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'second_chance_made'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'minus'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'plus'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'coach_tech_fouls']</t>
   </si>
 </sst>
 </file>
@@ -5634,7 +5799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A95B3A-52DF-1748-B037-EEA495CFFFA6}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R2" workbookViewId="0">
+    <sheetView topLeftCell="R2" workbookViewId="0">
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
@@ -6277,10 +6442,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8F9D3B-E9AA-B143-B309-156157DA3304}">
-  <dimension ref="B2:P82"/>
+  <dimension ref="B2:BU82"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N55" sqref="N22:N55"/>
+    <sheetView tabSelected="1" topLeftCell="AK43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB74" sqref="BB74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7139,7 +7304,7 @@
       </c>
       <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>27</v>
       </c>
@@ -7169,7 +7334,7 @@
       </c>
       <c r="P33" s="7"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>28</v>
       </c>
@@ -7199,7 +7364,7 @@
       </c>
       <c r="P34" s="7"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>29</v>
       </c>
@@ -7229,7 +7394,7 @@
       </c>
       <c r="P35" s="7"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>30</v>
       </c>
@@ -7259,7 +7424,7 @@
       </c>
       <c r="P36" s="7"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>31</v>
       </c>
@@ -7289,7 +7454,7 @@
       </c>
       <c r="P37" s="7"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
@@ -7319,7 +7484,7 @@
       </c>
       <c r="P38" s="7"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>33</v>
       </c>
@@ -7349,7 +7514,7 @@
       </c>
       <c r="P39" s="7"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>34</v>
       </c>
@@ -7378,8 +7543,173 @@
         <v>100</v>
       </c>
       <c r="P40" s="7"/>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S40" t="s">
+        <v>162</v>
+      </c>
+      <c r="T40" t="s">
+        <v>163</v>
+      </c>
+      <c r="U40" t="s">
+        <v>164</v>
+      </c>
+      <c r="V40" t="s">
+        <v>165</v>
+      </c>
+      <c r="W40" t="s">
+        <v>166</v>
+      </c>
+      <c r="X40" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>169</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>182</v>
+      </c>
+      <c r="AN40" t="s">
+        <v>183</v>
+      </c>
+      <c r="AO40" t="s">
+        <v>184</v>
+      </c>
+      <c r="AP40" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ40" t="s">
+        <v>186</v>
+      </c>
+      <c r="AR40" t="s">
+        <v>187</v>
+      </c>
+      <c r="AS40" t="s">
+        <v>188</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>189</v>
+      </c>
+      <c r="AU40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AV40" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW40" t="s">
+        <v>192</v>
+      </c>
+      <c r="AX40" t="s">
+        <v>193</v>
+      </c>
+      <c r="AY40" t="s">
+        <v>194</v>
+      </c>
+      <c r="AZ40" t="s">
+        <v>195</v>
+      </c>
+      <c r="BA40" t="s">
+        <v>196</v>
+      </c>
+      <c r="BB40" t="s">
+        <v>197</v>
+      </c>
+      <c r="BC40" t="s">
+        <v>198</v>
+      </c>
+      <c r="BD40" t="s">
+        <v>199</v>
+      </c>
+      <c r="BE40" t="s">
+        <v>200</v>
+      </c>
+      <c r="BF40" t="s">
+        <v>201</v>
+      </c>
+      <c r="BG40" t="s">
+        <v>202</v>
+      </c>
+      <c r="BH40" t="s">
+        <v>203</v>
+      </c>
+      <c r="BI40" t="s">
+        <v>204</v>
+      </c>
+      <c r="BJ40" t="s">
+        <v>205</v>
+      </c>
+      <c r="BK40" t="s">
+        <v>206</v>
+      </c>
+      <c r="BL40" t="s">
+        <v>207</v>
+      </c>
+      <c r="BM40" t="s">
+        <v>208</v>
+      </c>
+      <c r="BN40" t="s">
+        <v>209</v>
+      </c>
+      <c r="BO40" t="s">
+        <v>210</v>
+      </c>
+      <c r="BP40" t="s">
+        <v>211</v>
+      </c>
+      <c r="BQ40" t="s">
+        <v>212</v>
+      </c>
+      <c r="BR40" t="s">
+        <v>213</v>
+      </c>
+      <c r="BS40" t="s">
+        <v>214</v>
+      </c>
+      <c r="BT40" t="s">
+        <v>215</v>
+      </c>
+      <c r="BU40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>35</v>
       </c>
@@ -7409,7 +7739,7 @@
       </c>
       <c r="P41" s="7"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>36</v>
       </c>
@@ -7439,7 +7769,7 @@
       </c>
       <c r="P42" s="7"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>37</v>
       </c>
@@ -7469,7 +7799,7 @@
       </c>
       <c r="P43" s="7"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>38</v>
       </c>
@@ -7499,7 +7829,7 @@
       </c>
       <c r="P44" s="7"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>39</v>
       </c>
@@ -7529,7 +7859,7 @@
       </c>
       <c r="P45" s="7"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>40</v>
       </c>
@@ -7559,7 +7889,7 @@
       </c>
       <c r="P46" s="7"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>41</v>
       </c>
@@ -7589,7 +7919,7 @@
       </c>
       <c r="P47" s="7"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:73" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>58</v>
       </c>

</xml_diff>